<commit_message>
Validation tests added - all test executed under 3 minutes
</commit_message>
<xml_diff>
--- a/src/main/java/com/company/app/testdata/afsdata.xlsx
+++ b/src/main/java/com/company/app/testdata/afsdata.xlsx
@@ -27,42 +27,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>email</t>
   </si>
   <si>
-    <t>companyName</t>
-  </si>
-  <si>
     <t>phone</t>
   </si>
   <si>
     <t>9768787788</t>
   </si>
   <si>
-    <t>59786621</t>
-  </si>
-  <si>
-    <t>xpression2000</t>
-  </si>
-  <si>
-    <t>xpression2000@norway.com</t>
-  </si>
-  <si>
-    <t>eziport2000</t>
-  </si>
-  <si>
-    <t>eziport2000@norway.com</t>
-  </si>
-  <si>
     <t>msg</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>aa</t>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Alpha Romero</t>
+  </si>
+  <si>
+    <t>Beta Sedrik</t>
+  </si>
+  <si>
+    <t>Interested to work</t>
+  </si>
+  <si>
+    <t>+37259786621</t>
+  </si>
+  <si>
+    <t>xpression@test.com</t>
+  </si>
+  <si>
+    <t>arvotest@test.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t>Negative1</t>
+  </si>
+  <si>
+    <t>000000000</t>
+  </si>
+  <si>
+    <t>Hello World</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Negative2</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>abc@test.com</t>
+  </si>
+  <si>
+    <t>locate address?</t>
   </si>
 </sst>
 </file>
@@ -121,13 +145,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -409,31 +434,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.25" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" customWidth="1"/>
     <col min="3" max="3" width="16" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -441,35 +466,78 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="D3" s="6" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="xpression1000@norway.com"/>
-    <hyperlink ref="B3" r:id="rId2" display="eziport1000@norway.com"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B6" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>